<commit_message>
Retirados os números de filme dos textos.
</commit_message>
<xml_diff>
--- a/Listas.xlsx
+++ b/Listas.xlsx
@@ -2603,7 +2603,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F579"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A555" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A580" sqref="A580"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12476,7 +12479,8 @@
   <dimension ref="A1:G579"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Correção das tags do Homem de Ferro 2, nota de Elysium e manutenção da planilha.
</commit_message>
<xml_diff>
--- a/Listas.xlsx
+++ b/Listas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="45" windowWidth="20730" windowHeight="9975"/>
@@ -10,12 +10,15 @@
     <sheet name="Filmes" sheetId="1" r:id="rId1"/>
     <sheet name="Séries" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Filmes!$A$1:$F$582</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="591">
   <si>
     <t>#</t>
   </si>
@@ -1782,6 +1785,12 @@
   </si>
   <si>
     <t>se-puder-dirija</t>
+  </si>
+  <si>
+    <t>lovelace</t>
+  </si>
+  <si>
+    <t>elysium</t>
   </si>
 </sst>
 </file>
@@ -2604,20 +2613,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F580"/>
+  <dimension ref="A1:F582"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A570" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A580" sqref="A580"/>
+      <pane ySplit="1" topLeftCell="A553" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A582" sqref="A582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2627,10 +2637,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -12493,7 +12503,54 @@
         <v>2</v>
       </c>
     </row>
+    <row r="581" spans="1:6">
+      <c r="A581">
+        <v>580</v>
+      </c>
+      <c r="B581" t="s">
+        <v>589</v>
+      </c>
+      <c r="C581" s="1">
+        <v>41535</v>
+      </c>
+      <c r="D581" s="1">
+        <f>C581</f>
+        <v>41535</v>
+      </c>
+      <c r="E581">
+        <v>1</v>
+      </c>
+      <c r="F581">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6">
+      <c r="A582">
+        <v>581</v>
+      </c>
+      <c r="B582" t="s">
+        <v>590</v>
+      </c>
+      <c r="C582" s="1">
+        <v>41538</v>
+      </c>
+      <c r="D582" s="1">
+        <f>C582</f>
+        <v>41538</v>
+      </c>
+      <c r="E582">
+        <v>1</v>
+      </c>
+      <c r="F582">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F582">
+    <sortState ref="A2:F582">
+      <sortCondition ref="A1:A582"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Kung-Fusão Organização das litas.
</commit_message>
<xml_diff>
--- a/Listas.xlsx
+++ b/Listas.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="598">
   <si>
     <t>#</t>
   </si>
@@ -1791,6 +1791,27 @@
   </si>
   <si>
     <t>elysium</t>
+  </si>
+  <si>
+    <t>invocacao-do-mal</t>
+  </si>
+  <si>
+    <t>robocop-o-policial-do-futuro-1987</t>
+  </si>
+  <si>
+    <t>across-the-universe</t>
+  </si>
+  <si>
+    <t>a-familia</t>
+  </si>
+  <si>
+    <t>kung-fusao</t>
+  </si>
+  <si>
+    <t>breaking-bad</t>
+  </si>
+  <si>
+    <t>Nota Geral (1 a 5)</t>
   </si>
 </sst>
 </file>
@@ -2613,11 +2634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F582"/>
+  <dimension ref="A1:F587"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A553" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A582" sqref="A582"/>
+      <pane ySplit="1" topLeftCell="A565" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A587" sqref="A587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12543,6 +12564,111 @@
       </c>
       <c r="F582">
         <v>3</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6">
+      <c r="A583">
+        <v>582</v>
+      </c>
+      <c r="B583" t="s">
+        <v>591</v>
+      </c>
+      <c r="C583" s="1">
+        <v>41543</v>
+      </c>
+      <c r="D583" s="1">
+        <f>C583</f>
+        <v>41543</v>
+      </c>
+      <c r="E583">
+        <v>1</v>
+      </c>
+      <c r="F583">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6">
+      <c r="A584">
+        <v>583</v>
+      </c>
+      <c r="B584" t="s">
+        <v>592</v>
+      </c>
+      <c r="C584" s="1">
+        <v>41544</v>
+      </c>
+      <c r="D584" s="1">
+        <f>C584</f>
+        <v>41544</v>
+      </c>
+      <c r="E584">
+        <v>1</v>
+      </c>
+      <c r="F584">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6">
+      <c r="A585">
+        <v>584</v>
+      </c>
+      <c r="B585" t="s">
+        <v>593</v>
+      </c>
+      <c r="C585" s="1">
+        <v>41545</v>
+      </c>
+      <c r="D585" s="1">
+        <f>C585</f>
+        <v>41545</v>
+      </c>
+      <c r="E585">
+        <v>1</v>
+      </c>
+      <c r="F585">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6">
+      <c r="A586">
+        <v>585</v>
+      </c>
+      <c r="B586" t="s">
+        <v>594</v>
+      </c>
+      <c r="C586" s="1">
+        <v>41551</v>
+      </c>
+      <c r="D586" s="1">
+        <f>C586</f>
+        <v>41551</v>
+      </c>
+      <c r="E586">
+        <v>1</v>
+      </c>
+      <c r="F586">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6">
+      <c r="A587">
+        <v>586</v>
+      </c>
+      <c r="B587" t="s">
+        <v>595</v>
+      </c>
+      <c r="C587" s="1">
+        <v>41553</v>
+      </c>
+      <c r="D587" s="1">
+        <f>C587</f>
+        <v>41553</v>
+      </c>
+      <c r="E587">
+        <v>1</v>
+      </c>
+      <c r="F587">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12571,7 +12697,7 @@
     <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -12594,7 +12720,7 @@
         <v>587</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -12608,7 +12734,7 @@
         <v>41336</v>
       </c>
       <c r="D2" s="1">
-        <v>41336</v>
+        <v>41367</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -12634,18 +12760,37 @@
         <v>41462</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41061</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41547</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
Pequenas correções nas cotações e detalhes dos curtas.
</commit_message>
<xml_diff>
--- a/Listas.xlsx
+++ b/Listas.xlsx
@@ -2806,7 +2806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A571" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F594" sqref="F594"/>
+      <selection pane="bottomLeft" activeCell="F593" sqref="F593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12941,7 +12941,7 @@
         <v>1</v>
       </c>
       <c r="F592">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="593" spans="1:6">

</xml_diff>